<commit_message>
Updated Readme.md (other steps).
</commit_message>
<xml_diff>
--- a/doc/Signature/SignatureTestData.xlsx
+++ b/doc/Signature/SignatureTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Playground\ImageProcessing.marko\doc\Signature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E729D0-1872-41F6-8D9C-80AAF08B2FFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4940D791-06C9-417E-8FA8-0F61AADE41C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -110,8 +110,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -204,15 +204,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -230,6 +230,2045 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>53228</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>2802</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114860</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>2802</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C32C8DE-95F7-4F01-8BC0-81D0FB481DB9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="972110" y="6535831"/>
+          <a:ext cx="980515" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>148828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>53578</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6131FD1A-5E9E-46B1-B738-2F8DB27004E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1312070" y="5923359"/>
+          <a:ext cx="1226344" cy="1238250"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6F085F-E20B-4147-BF62-C97039BE2305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1304925" y="7543800"/>
+          <a:ext cx="1276350" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Isosceles Triangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDAF0DCB-69A1-4582-BF46-F02F347CAC00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1333500" y="8753475"/>
+          <a:ext cx="1238250" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="triangle">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>164782</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>53578</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="Group 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{905F4074-9634-4E26-AF30-B613A35A5A7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1897380" y="6484620"/>
+          <a:ext cx="96202" cy="103108"/>
+          <a:chOff x="1906345" y="6483499"/>
+          <a:chExt cx="96202" cy="103108"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="6" name="Straight Connector 5">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1AF277B-8487-4F26-890A-A4F74154153D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1956827" y="6483499"/>
+            <a:ext cx="0" cy="103108"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="7" name="Straight Connector 6">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64762AC2-2845-414D-804C-C9D1DE3F85FC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="1906345" y="6533029"/>
+            <a:ext cx="96202" cy="1667"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>169494</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>33618</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>42026</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>86845</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Arc 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A4C861A-4349-499A-AF6A-F49379176843}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="1115690" y="5777333"/>
+          <a:ext cx="1196227" cy="1250856"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16289508"/>
+            <a:gd name="adj2" fmla="val 150026"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>44825</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106457</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>100852</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8969EC8A-A94B-4DB1-AB66-CBDD2ACBB517}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="963707" y="7967381"/>
+          <a:ext cx="980515" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>60177</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>48520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>156379</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>151628</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="15" name="Group 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3779DF61-057C-4648-9F00-7122CDEE1705}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1888977" y="7916170"/>
+          <a:ext cx="96202" cy="103108"/>
+          <a:chOff x="1906345" y="6483499"/>
+          <a:chExt cx="96202" cy="103108"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="Straight Connector 15">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C8B7179-0EE3-46D2-A1E7-BC63FEE5F47E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1956827" y="6483499"/>
+            <a:ext cx="0" cy="103108"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="17" name="Straight Connector 16">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C933F38-E320-4ED1-B325-7D0BE98E87EF}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="1906345" y="6533029"/>
+            <a:ext cx="96202" cy="1667"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161091</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>42023</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>184895</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Arc 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749C5F3F-B92F-4D43-A38D-3684DD2B9C10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="857954" y="7640312"/>
+          <a:ext cx="1014131" cy="570094"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16289508"/>
+            <a:gd name="adj2" fmla="val 150026"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50428</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>154081</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>112060</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>154081</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{960216EE-E73A-48F9-A39F-09B396492AE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="969310" y="9354110"/>
+          <a:ext cx="980515" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>65780</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>101749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161982</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>14357</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="20" name="Group 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CE166FD-A4A2-45BD-B1B2-809E87B9A807}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1894580" y="9302899"/>
+          <a:ext cx="96202" cy="103108"/>
+          <a:chOff x="1906345" y="6483499"/>
+          <a:chExt cx="96202" cy="103108"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="21" name="Straight Connector 20">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6360D826-79BC-4C75-BEFA-A9793CF5A9D3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1956827" y="6483499"/>
+            <a:ext cx="0" cy="103108"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="22" name="Straight Connector 21">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{570AB4F8-FADD-4B0C-8310-702EA59BE26A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1" flipV="1">
+            <a:off x="1906345" y="6533029"/>
+            <a:ext cx="96202" cy="1667"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>166694</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>184897</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>39226</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Arc 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CABA4B0-A353-4F37-9D07-5D73F6E26313}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="1112890" y="8595612"/>
+          <a:ext cx="1196227" cy="1250856"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16289508"/>
+            <a:gd name="adj2" fmla="val 150026"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>203489</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>25977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>203489</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>90921</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD2B2664-BFDB-46D0-9333-2BBF28A245BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3251489" y="5987761"/>
+          <a:ext cx="0" cy="1017444"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>199159</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>90920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>82261</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>90920</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89719B55-E7AB-494B-9395-B1D9DAE0574C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3247159" y="7005204"/>
+          <a:ext cx="2407227" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>48490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>181841</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Connector 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C3F633-6F7E-45CD-94D4-AE36B880DFEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3248025" y="6391274"/>
+          <a:ext cx="2047009" cy="3465"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>199160</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>90921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>199160</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>155865</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C76DB866-EB8A-4D4E-A7C1-AE62BF7C6A80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3247160" y="7386205"/>
+          <a:ext cx="0" cy="1017444"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>194830</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>77932</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Straight Connector 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{137CE3B1-A1D2-4DC2-AB88-338E5AE06E17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3242830" y="8403648"/>
+          <a:ext cx="2407227" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>162109</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123009</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>43041</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>184640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Arc 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69A32F77-149E-4937-9EE2-9C861324F341}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="857572" y="7640694"/>
+          <a:ext cx="1014131" cy="569329"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16289508"/>
+            <a:gd name="adj2" fmla="val 150026"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>223232</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>126299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>672</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>116898</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="62" name="Group 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99EE99D8-9736-46C7-9C0D-4DF7B939334A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3261707" y="7041449"/>
+          <a:ext cx="2292040" cy="1133599"/>
+          <a:chOff x="3271232" y="7040583"/>
+          <a:chExt cx="2301565" cy="1002683"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="56" name="Arc 55">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{830B99E7-158B-457B-85B8-0D2D98F8AFED}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="6649172">
+            <a:off x="3187418" y="7414389"/>
+            <a:ext cx="362786" cy="195158"/>
+          </a:xfrm>
+          <a:prstGeom prst="arc">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 16212781"/>
+              <a:gd name="adj2" fmla="val 972189"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:endParaRPr lang="de-CH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="57" name="Arc 56">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD287C7B-7DC0-42F2-A141-C32F6DDB6617}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="3456327" y="7044047"/>
+            <a:ext cx="687048" cy="999219"/>
+          </a:xfrm>
+          <a:prstGeom prst="arc">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 10708402"/>
+              <a:gd name="adj2" fmla="val 104848"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:endParaRPr lang="de-CH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="58" name="Arc 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8BEF9DC-6698-465A-B0C1-8B5789D866D8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="4154250" y="7359637"/>
+            <a:ext cx="326830" cy="327487"/>
+          </a:xfrm>
+          <a:prstGeom prst="arc">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 10905747"/>
+              <a:gd name="adj2" fmla="val 21541669"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:endParaRPr lang="de-CH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="59" name="Arc 58">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C32AAD7-4B2C-4B6E-B965-9F0A0626813B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000">
+            <a:off x="4483295" y="7040583"/>
+            <a:ext cx="687048" cy="999219"/>
+          </a:xfrm>
+          <a:prstGeom prst="arc">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 10708402"/>
+              <a:gd name="adj2" fmla="val 104848"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:endParaRPr lang="de-CH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="60" name="Arc 59">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE5C8E59-4F26-4E7D-91E1-2849DE15C755}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="13499403">
+            <a:off x="5125395" y="7552192"/>
+            <a:ext cx="447402" cy="173639"/>
+          </a:xfrm>
+          <a:prstGeom prst="arc">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 17377551"/>
+              <a:gd name="adj2" fmla="val 21033319"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="l"/>
+            <a:endParaRPr lang="de-CH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>205242</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>46883</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>205242</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>111827</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Straight Connector 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99D9530A-5C3B-46A2-9602-5D4CEB4441C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3253242" y="8675667"/>
+          <a:ext cx="0" cy="1017444"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200912</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>111826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>84014</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>111826</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Connector 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{207B7151-2F9E-48B5-8916-A184F24874DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3248912" y="9693110"/>
+          <a:ext cx="2407227" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="arrow" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>218901</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>129886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>95248</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>43293</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="71" name="Arc 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAC49E4B-B2ED-4E55-A6FC-1EE37587EC39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="3496367" y="8568170"/>
+          <a:ext cx="794211" cy="675407"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 10708402"/>
+            <a:gd name="adj2" fmla="val 104848"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>98540</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>135082</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>204354</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>48489</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Arc 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEAE036F-0108-4720-93C5-AF0C5F88E2F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="4293870" y="8573366"/>
+          <a:ext cx="794211" cy="675407"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 10708402"/>
+            <a:gd name="adj2" fmla="val 104848"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>207819</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>129887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>84166</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>43294</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Arc 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F255D0D9-E844-44F2-8263-528F2D2796A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5091546" y="8568171"/>
+          <a:ext cx="794211" cy="675407"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18269118"/>
+            <a:gd name="adj2" fmla="val 104848"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>412174</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>135083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>223578</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>48490</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Arc 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C372A1CD-EB6A-45ED-8254-0B9DCBB2E850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2706833" y="8573367"/>
+          <a:ext cx="794211" cy="675407"/>
+        </a:xfrm>
+        <a:prstGeom prst="arc">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 10661096"/>
+            <a:gd name="adj2" fmla="val 14708908"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:srgbClr val="00B050"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-CH" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -497,8 +2536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AD24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,11 +2646,11 @@
         <f>AA13*$AB$10</f>
         <v>0</v>
       </c>
-      <c r="AC13" s="11">
+      <c r="AC13" s="9">
         <f>SIN(AB13)</f>
         <v>0</v>
       </c>
-      <c r="AD13" s="11">
+      <c r="AD13" s="9">
         <f>COS(AB13)</f>
         <v>1</v>
       </c>
@@ -636,11 +2675,11 @@
         <f t="shared" ref="AB14" si="0">AA14*$AB$10</f>
         <v>0.52359877559829837</v>
       </c>
-      <c r="AC14" s="11">
+      <c r="AC14" s="9">
         <f t="shared" ref="AC14" si="1">SIN(AB14)</f>
         <v>0.49999999999999956</v>
       </c>
-      <c r="AD14" s="11">
+      <c r="AD14" s="9">
         <f t="shared" ref="AD14" si="2">COS(AB14)</f>
         <v>0.86602540378443893</v>
       </c>
@@ -661,15 +2700,15 @@
         <v>45</v>
       </c>
       <c r="AB15" s="8">
-        <f t="shared" ref="AB15:AB22" si="3">AA15*$AB$10</f>
+        <f t="shared" ref="AB15:AB16" si="3">AA15*$AB$10</f>
         <v>0.7853981633974475</v>
       </c>
-      <c r="AC15" s="11">
-        <f t="shared" ref="AC15:AC22" si="4">SIN(AB15)</f>
+      <c r="AC15" s="9">
+        <f t="shared" ref="AC15:AC16" si="4">SIN(AB15)</f>
         <v>0.70710678118654691</v>
       </c>
-      <c r="AD15" s="11">
-        <f t="shared" ref="AD15:AD22" si="5">COS(AB15)</f>
+      <c r="AD15" s="9">
+        <f t="shared" ref="AD15:AD16" si="5">COS(AB15)</f>
         <v>0.70710678118654813</v>
       </c>
     </row>
@@ -689,11 +2728,11 @@
         <f t="shared" si="3"/>
         <v>1.0471975511965967</v>
       </c>
-      <c r="AC16" s="11">
+      <c r="AC16" s="9">
         <f t="shared" si="4"/>
         <v>0.86602540378443815</v>
       </c>
-      <c r="AD16" s="11">
+      <c r="AD16" s="9">
         <f t="shared" si="5"/>
         <v>0.50000000000000089</v>
       </c>
@@ -706,15 +2745,15 @@
         <v>90</v>
       </c>
       <c r="AB17" s="8">
-        <f>AA17*$AB$10</f>
+        <f t="shared" ref="AB17:AB23" si="6">AA17*$AB$10</f>
         <v>1.570796326794895</v>
       </c>
-      <c r="AC17" s="11">
-        <f>SIN(AB17)</f>
+      <c r="AC17" s="9">
+        <f t="shared" ref="AC17:AC23" si="7">SIN(AB17)</f>
         <v>1</v>
       </c>
-      <c r="AD17" s="11">
-        <f>COS(AB17)</f>
+      <c r="AD17" s="9">
+        <f t="shared" ref="AD17:AD23" si="8">COS(AB17)</f>
         <v>1.6155696572206502E-15</v>
       </c>
     </row>
@@ -723,15 +2762,15 @@
         <v>135</v>
       </c>
       <c r="AB18" s="8">
-        <f>AA18*$AB$10</f>
+        <f t="shared" si="6"/>
         <v>2.3561944901923426</v>
       </c>
-      <c r="AC18" s="11">
-        <f>SIN(AB18)</f>
+      <c r="AC18" s="9">
+        <f t="shared" si="7"/>
         <v>0.70710678118654913</v>
       </c>
-      <c r="AD18" s="11">
-        <f>COS(AB18)</f>
+      <c r="AD18" s="9">
+        <f t="shared" si="8"/>
         <v>-0.70710678118654591</v>
       </c>
     </row>
@@ -739,22 +2778,22 @@
       <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="11">
         <v>0</v>
       </c>
-      <c r="E19" s="9"/>
+      <c r="E19" s="11"/>
       <c r="G19" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="12">
+      <c r="I19" s="12"/>
+      <c r="J19" s="10">
         <f>COS(D21)</f>
         <v>-1</v>
       </c>
-      <c r="K19" s="12"/>
+      <c r="K19" s="10"/>
       <c r="M19">
         <v>-1</v>
       </c>
@@ -762,15 +2801,15 @@
         <v>180</v>
       </c>
       <c r="AB19" s="8">
-        <f>AA19*$AB$10</f>
+        <f t="shared" si="6"/>
         <v>3.14159265358979</v>
       </c>
-      <c r="AC19" s="11">
-        <f>SIN(AB19)</f>
+      <c r="AC19" s="9">
+        <f t="shared" si="7"/>
         <v>3.2311393144413003E-15</v>
       </c>
-      <c r="AD19" s="11">
-        <f>COS(AB19)</f>
+      <c r="AD19" s="9">
+        <f t="shared" si="8"/>
         <v>-1</v>
       </c>
     </row>
@@ -778,23 +2817,23 @@
       <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="11">
         <f>D19+180</f>
         <v>180</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="11"/>
       <c r="G20" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="12">
+      <c r="I20" s="12"/>
+      <c r="J20" s="10">
         <f>SIN(D21)</f>
         <v>3.2311393144413003E-15</v>
       </c>
-      <c r="K20" s="12"/>
+      <c r="K20" s="10"/>
       <c r="M20">
         <v>0</v>
       </c>
@@ -802,15 +2841,15 @@
         <v>225</v>
       </c>
       <c r="AB20" s="8">
-        <f>AA20*$AB$10</f>
+        <f t="shared" si="6"/>
         <v>3.9269908169872374</v>
       </c>
-      <c r="AC20" s="11">
-        <f>SIN(AB20)</f>
+      <c r="AC20" s="9">
+        <f t="shared" si="7"/>
         <v>-0.70710678118654458</v>
       </c>
-      <c r="AD20" s="11">
-        <f>COS(AB20)</f>
+      <c r="AD20" s="9">
+        <f t="shared" si="8"/>
         <v>-0.70710678118655046</v>
       </c>
     </row>
@@ -818,24 +2857,24 @@
       <c r="B21" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="11">
         <f>D20*AB10</f>
         <v>3.14159265358979</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="11"/>
       <c r="AA21" s="7">
         <v>270</v>
       </c>
       <c r="AB21" s="8">
-        <f>AA21*$AB$10</f>
+        <f t="shared" si="6"/>
         <v>4.7123889803846852</v>
       </c>
-      <c r="AC21" s="11">
-        <f>SIN(AB21)</f>
+      <c r="AC21" s="9">
+        <f t="shared" si="7"/>
         <v>-1</v>
       </c>
-      <c r="AD21" s="11">
-        <f>COS(AB21)</f>
+      <c r="AD21" s="9">
+        <f t="shared" si="8"/>
         <v>-4.6246643667369192E-15</v>
       </c>
     </row>
@@ -844,37 +2883,37 @@
         <v>315</v>
       </c>
       <c r="AB22" s="8">
-        <f>AA22*$AB$10</f>
+        <f t="shared" si="6"/>
         <v>5.4977871437821326</v>
       </c>
-      <c r="AC22" s="11">
-        <f>SIN(AB22)</f>
+      <c r="AC22" s="9">
+        <f t="shared" si="7"/>
         <v>-0.70710678118655146</v>
       </c>
-      <c r="AD22" s="11">
-        <f>COS(AB22)</f>
+      <c r="AD22" s="9">
+        <f t="shared" si="8"/>
         <v>0.70710678118654358</v>
       </c>
     </row>
     <row r="23" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="D23" s="9">
+      <c r="D23" s="11">
         <f>D20/360</f>
         <v>0.5</v>
       </c>
-      <c r="E23" s="9"/>
+      <c r="E23" s="11"/>
       <c r="AA23" s="7">
         <v>360</v>
       </c>
       <c r="AB23" s="8">
-        <f>AA23*$AB$10</f>
+        <f t="shared" si="6"/>
         <v>6.28318530717958</v>
       </c>
-      <c r="AC23" s="11">
-        <f>SIN(AB23)</f>
+      <c r="AC23" s="9">
+        <f t="shared" si="7"/>
         <v>-6.4622786288826006E-15</v>
       </c>
-      <c r="AD23" s="11">
-        <f>COS(AB23)</f>
+      <c r="AD23" s="9">
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
     </row>
@@ -882,14 +2921,14 @@
       <c r="B24" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="12">
         <v>3.14159265358979</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -905,5 +2944,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>